<commit_message>
Add UNPD filename replacement and improve INCHIKEY matching
This commit adds a new filename replacement for 'UNPD' in the dataframe processing and improves handling of missing INCHIKEY matches. It handles exceptions by providing an empty string when there's no match with the regular expression pattern, making INCHIKEY processing more robust. The changes also include printing of both original and pivoted data frames for debug purposes.
</commit_message>
<xml_diff>
--- a/datas/BENCHMARK.xlsx
+++ b/datas/BENCHMARK.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t xml:space="preserve">MATCHMS</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t xml:space="preserve">TOTAL TIME :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--- TOTAL TIME: 02:24:04 ---</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -816,7 +819,9 @@
       <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="E23" s="3" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Update dataframe processing logic for filename and INCHIKEY
The commit modifies the dataframe processing routine to substitute 'UNPD' filenames. It also refines INCHIKEY matching mechanism and ensures that it returns an empty string when no matches are found. Lastly, it contains improvements on both the original and pivoted dataframes.
</commit_message>
<xml_diff>
--- a/datas/BENCHMARK.xlsx
+++ b/datas/BENCHMARK.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t xml:space="preserve">MATCHMS</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t xml:space="preserve">--- TOTAL TIME: 02:24:04 ---</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--- TOTAL TIME: 00:23:27 ---</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -826,7 +829,9 @@
       <c r="E23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="G23" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update generate_colors_dict.py to simplify color generation
The color generation process in generate_colors_dict.py has been simplified by using 'colorsys' and 'colors' modules from matplotlib. The method for conversion of colors has been streamlined, and the list of categories has been reviewed and cleaned up. This refactoring will make the code more maintainable and easier to understand.
</commit_message>
<xml_diff>
--- a/datas/BENCHMARK.xlsx
+++ b/datas/BENCHMARK.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
   <si>
     <t xml:space="preserve">MATCHMS</t>
   </si>
@@ -43,85 +43,157 @@
     <t xml:space="preserve">MoNA-export-Experimental_Spectra.msp</t>
   </si>
   <si>
-    <t xml:space="preserve">1,25 Go</t>
-  </si>
-  <si>
     <t xml:space="preserve">MoNA-export-Experimental_Spectra.json</t>
   </si>
   <si>
-    <t xml:space="preserve">3,04 Go</t>
+    <t xml:space="preserve">MassBank_NIST.msp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MassBank_RIKEN.msp</t>
   </si>
   <si>
     <t xml:space="preserve">MSMS_Public_ExpBioInsilico_NEG_VS17.msp</t>
   </si>
   <si>
-    <t xml:space="preserve">51,3 Mo</t>
-  </si>
-  <si>
     <t xml:space="preserve">MSMS_Public_ExpBioInsilico_Pos_VS17.msp</t>
   </si>
   <si>
-    <t xml:space="preserve">259 Mo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MassBank_NIST.msp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">95,1 Mo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MassBank_RIKEN.msp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">114 Mo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALL_GNPS.json</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,79 Go</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNPD_ISDB_R_p01_predicted.mgf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48,8 Mo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNPD_ISDB_R_p02_predicted.mgf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNPD_ISDB_R_p03_predicted.mgf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNPD_ISDB_R_p04_predicted.mgf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNPD_ISDB_R_p05_predicted.mgf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNPD_ISDB_R_p06_predicted.mgf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNPD_ISDB_R_p07_predicted.mgf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNPD_ISDB_R_p08_predicted.mgf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNPD_ISDB_R_p09_predicted.mgf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47,8 Mo</t>
+    <t xml:space="preserve">BERKELEY-LAB.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BILELIB19.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEREPLICATOR_IDENTIFIED_LIBRARY.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRUGS-OF-ABUSE-LIBRARY.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECG-ACYL-AMIDES-C4-C24-LIBRARY.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECG-ACYL-ESTERS-C4-C24-LIBRARY.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-COLLECTIONS-MISC.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-COLLECTIONS-PESTICIDES-NEGATIVE.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-COLLECTIONS-PESTICIDES-POSITIVE.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-D2-AMINO-LIPID-LIBRARY.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-EMBL-MCF.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-FAULKNERLEGACY.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-IOBA-NHC.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-LIBRARY.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-NIH-CLINICALCOLLECTION1.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-NIH-CLINICALCOLLECTION2.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-NIH-NATURALPRODUCTSLIBRARY.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-NIH-NATURALPRODUCTSLIBRARY_ROUND2_NEGATIVE.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-NIH-NATURALPRODUCTSLIBRARY_ROUND2_POSITIVE.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-NIH-SMALLMOLECULEPHARMACOLOGICALLYACTIVE.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-NIST14-MATCHES.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-NUTRI-METAB-FEM-NEG.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-NUTRI-METAB-FEM-POS.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-PRESTWICKPHYTOCHEM.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-SAM-SIK-KANG-LEGACY-LIBRARY.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-SCIEX-LIBRARY.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-SELLECKCHEM-FDA-PART1.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-SELLECKCHEM-FDA-PART2.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCE-CELL-LYSATE-LIPIDS.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IQAMDB.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDB_NEGATIVE.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDB_POSITIVE.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEAFBOT.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIADB.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMV_NEGATIVE.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMV_POSITIVE.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEO-MSMS.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PNNL-LIPIDS-NEGATIVE.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PNNL-LIPIDS-POSITIVE.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSU-MSMLS.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TUEBINGEN-NATURAL-PRODUCT-COLLECTION.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UM-NPDC.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XANTHONES-DB.mgf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNPS-MSMLS.mgf</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL TIME :</t>
   </si>
   <si>
-    <t xml:space="preserve">--- TOTAL TIME: 02:24:04 ---</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--- TOTAL TIME: 00:23:27 ---</t>
+    <t xml:space="preserve">--- TOTAL TIME: 00:11:07 ---</t>
   </si>
 </sst>
 </file>
@@ -216,7 +288,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,6 +306,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -486,21 +574,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="33.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="36.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="53.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="53.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,12 +595,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -522,317 +607,535 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="B22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="E23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="3" t="s">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="3"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="7"/>
+      <c r="B52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="0"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="0"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="7"/>
+      <c r="D54" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Refactor color generation in generate_colors_dict.py
The updated generate_colors_dict.py utilizes 'colorsys' and 'colors' modules from matplotlib to simplify the color generation process. The refactoring has streamlined color conversions and revised the category list, enhancing the code's maintainability and readability.
</commit_message>
<xml_diff>
--- a/datas/BENCHMARK.xlsx
+++ b/datas/BENCHMARK.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t xml:space="preserve">MATCHMS</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t xml:space="preserve">TOTAL TIME :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--- TOTAL TIME: 01:49:57 ---</t>
   </si>
   <si>
     <t xml:space="preserve">--- TOTAL TIME: 00:11:07 ---</t>
@@ -577,7 +580,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
+      <selection pane="topLeft" activeCell="D57" activeCellId="0" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1129,12 +1132,14 @@
       <c r="A54" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="7"/>
+      <c r="B54" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="D54" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>